<commit_message>
Remove unnecessary information in templates
</commit_message>
<xml_diff>
--- a/public/data/templates/ICGLR-packing-list.xlsx
+++ b/public/data/templates/ICGLR-packing-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WebStormProjects\mining-company-management-system-backend\public\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141BF90D-DBF3-47A4-9253-3BBF13CF5984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5868D2DC-5365-4DB1-AC0E-4BF365F7C5D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">TYPE OF MINERAL TO BE EXPORTED:WOLFRAM                         </t>
-  </si>
   <si>
     <t>RESERVED FOR ALL TYPES OF MINERALS</t>
   </si>
@@ -118,16 +115,19 @@
     <t>EXPORTER NAME: KANZAMIN LIMITED</t>
   </si>
   <si>
-    <t>ITRI/iTSCi SHIPMENT NUMBER: KZM/RW/0000022</t>
+    <t xml:space="preserve">TYPE OF MINERAL TO BE EXPORTED:                         </t>
   </si>
   <si>
-    <t>LOT NUMBER: WKKIG2303</t>
+    <t xml:space="preserve">ITRI/iTSCi SHIPMENT NUMBER: </t>
   </si>
   <si>
-    <t>APPLICATION DATE: 16/11/2023</t>
+    <t xml:space="preserve">LOT NUMBER: </t>
   </si>
   <si>
-    <t>ANTICIPATED SHIPMENT DATE: 20/11/2023</t>
+    <t xml:space="preserve">APPLICATION DATE: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTICIPATED SHIPMENT DATE: </t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -444,7 +444,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -534,6 +534,36 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -563,36 +593,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,15 +999,15 @@
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
-        <v>31</v>
+      <c r="A2" s="70" t="s">
+        <v>30</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="5"/>
@@ -1029,15 +1029,15 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>0</v>
+      <c r="A3" s="70" t="s">
+        <v>31</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="62"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="5"/>
@@ -1059,15 +1059,15 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="72"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" s="5"/>
@@ -1089,15 +1089,15 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="62"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="72"/>
       <c r="H5" s="5"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -1119,15 +1119,15 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
       <c r="H6" s="5"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -1149,15 +1149,15 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="72"/>
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
@@ -1207,115 +1207,115 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="67" t="s">
+      <c r="N9" s="78"/>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="70" t="s">
+      <c r="T9" s="61"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="T9" s="71"/>
-      <c r="U9" s="72"/>
-      <c r="V9" s="73" t="s">
+      <c r="W9" s="64"/>
+      <c r="X9" s="65"/>
+      <c r="Y9" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="W9" s="74"/>
-      <c r="X9" s="75"/>
-      <c r="Y9" s="76" t="s">
+      <c r="Z9" s="67"/>
+    </row>
+    <row r="10" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="Z9" s="77"/>
-    </row>
-    <row r="10" spans="1:26" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="D10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="F10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="I10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="J10" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="K10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="L10" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="47" t="s">
+      <c r="M10" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="78" t="s">
+      <c r="N10" s="69"/>
+      <c r="O10" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="79"/>
-      <c r="O10" s="78" t="s">
+      <c r="P10" s="69"/>
+      <c r="Q10" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="78" t="s">
+      <c r="R10" s="69"/>
+      <c r="S10" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="79"/>
-      <c r="S10" s="49" t="s">
+      <c r="T10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="T10" s="25" t="s">
+      <c r="U10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="U10" s="26" t="s">
+      <c r="V10" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="V10" s="26" t="s">
+      <c r="W10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="W10" s="26" t="s">
+      <c r="X10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="X10" s="26" t="s">
+      <c r="Y10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="Y10" s="26" t="s">
+      <c r="Z10" s="27" t="s">
         <v>27</v>
-      </c>
-      <c r="Z10" s="27" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1332,22 +1332,22 @@
       <c r="K11" s="34"/>
       <c r="L11" s="48"/>
       <c r="M11" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="35" t="s">
-        <v>30</v>
+      <c r="O11" s="35" t="s">
+        <v>28</v>
       </c>
-      <c r="O11" s="35" t="s">
+      <c r="P11" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="35" t="s">
-        <v>30</v>
-      </c>
       <c r="Q11" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R11" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S11" s="58"/>
       <c r="T11" s="43"/>
@@ -15777,12 +15777,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="M9:R9"/>
@@ -15791,6 +15785,12 @@
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>